<commit_message>
Update of 2025 data and RF changes
</commit_message>
<xml_diff>
--- a/OnBoard/output/trust/catch/Catch_Trust_1.xlsx
+++ b/OnBoard/output/trust/catch/Catch_Trust_1.xlsx
@@ -1190,7 +1190,7 @@
         <v>99</v>
       </c>
       <c r="I20">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="21">
@@ -1231,7 +1231,7 @@
         <v>26</v>
       </c>
       <c r="I21">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="22">
@@ -1272,7 +1272,7 @@
         <v>11</v>
       </c>
       <c r="I22">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="23">
@@ -1313,7 +1313,7 @@
         <v>41</v>
       </c>
       <c r="I23">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="24">
@@ -1354,7 +1354,7 @@
         <v>111</v>
       </c>
       <c r="I24">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="25">
@@ -1395,7 +1395,7 @@
         <v>-1</v>
       </c>
       <c r="I25">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="26">
@@ -1436,7 +1436,7 @@
         <v>114</v>
       </c>
       <c r="I26">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="27">
@@ -1477,7 +1477,7 @@
         <v>2</v>
       </c>
       <c r="I27">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="28">
@@ -1518,7 +1518,7 @@
         <v>4</v>
       </c>
       <c r="I28">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="29">
@@ -1559,7 +1559,7 @@
         <v>-1</v>
       </c>
       <c r="I29">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="30">
@@ -1600,7 +1600,7 @@
         <v>1</v>
       </c>
       <c r="I30">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="31">
@@ -1641,7 +1641,7 @@
         <v>1</v>
       </c>
       <c r="I31">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="32">
@@ -1682,7 +1682,7 @@
         <v>2</v>
       </c>
       <c r="I32">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="33">
@@ -1723,7 +1723,7 @@
         <v>23</v>
       </c>
       <c r="I33">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="34">
@@ -1764,7 +1764,7 @@
         <v>1</v>
       </c>
       <c r="I34">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="35">
@@ -1805,7 +1805,7 @@
         <v>1</v>
       </c>
       <c r="I35">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="36">
@@ -1846,7 +1846,7 @@
         <v>2</v>
       </c>
       <c r="I36">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="37">
@@ -1887,7 +1887,7 @@
         <v>11</v>
       </c>
       <c r="I37">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="38">
@@ -1928,7 +1928,7 @@
         <v>3</v>
       </c>
       <c r="I38">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="39">
@@ -1969,7 +1969,7 @@
         <v>167</v>
       </c>
       <c r="I39">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="40">
@@ -2010,7 +2010,7 @@
         <v>1</v>
       </c>
       <c r="I40">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="41">
@@ -2051,7 +2051,7 @@
         <v>14</v>
       </c>
       <c r="I41">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="42">
@@ -2092,7 +2092,7 @@
         <v>61</v>
       </c>
       <c r="I42">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="43">
@@ -2133,7 +2133,7 @@
         <v>2</v>
       </c>
       <c r="I43">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="44">
@@ -2174,7 +2174,7 @@
         <v>9</v>
       </c>
       <c r="I44">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="45">
@@ -2215,7 +2215,7 @@
         <v>5</v>
       </c>
       <c r="I45">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="46">
@@ -2256,7 +2256,7 @@
         <v>1</v>
       </c>
       <c r="I46">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="47">
@@ -2297,7 +2297,7 @@
         <v>168</v>
       </c>
       <c r="I47">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="48">
@@ -2338,7 +2338,7 @@
         <v>-1</v>
       </c>
       <c r="I48">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="49">
@@ -2379,7 +2379,7 @@
         <v>7</v>
       </c>
       <c r="I49">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="50">
@@ -2420,7 +2420,7 @@
         <v>-1</v>
       </c>
       <c r="I50">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="51">
@@ -2461,7 +2461,7 @@
         <v>3</v>
       </c>
       <c r="I51">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="52">
@@ -2502,7 +2502,7 @@
         <v>1</v>
       </c>
       <c r="I52">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
     <row r="53">
@@ -2543,7 +2543,7 @@
         <v>-1</v>
       </c>
       <c r="I53">
-        <v>28.23277777777777</v>
+        <v>11.95527272727273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>